<commit_message>
Agrega resultados de reglas empíricas para periodos de 90 días
</commit_message>
<xml_diff>
--- a/experimentos/comparacion_experimentos.xlsx
+++ b/experimentos/comparacion_experimentos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Exceso_sobre_BH" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Ganancia_Total" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Exceso_sobre_BH_90" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ganancia_Total_90" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="46">
   <si>
     <t>Periodo Prueba</t>
   </si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>Máxima pérdida (Anualizada – por cada 100 mil pesos)</t>
+  </si>
+  <si>
+    <t>Reglas empíricas</t>
+  </si>
+  <si>
+    <t>Yo_resultados</t>
+  </si>
+  <si>
+    <t>AQ_exp_1_2</t>
+  </si>
+  <si>
+    <t>CN2_exp_1_2</t>
+  </si>
+  <si>
+    <t>Ganancia Total</t>
   </si>
   <si>
     <t>Promedio (Anualizado – Decimal, dividido entre 100 mil)</t>
@@ -155,11 +170,12 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -177,15 +193,11 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -197,14 +209,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FF66"/>
-        <bgColor rgb="FF99CC00"/>
+        <fgColor rgb="FF00CC33"/>
+        <bgColor rgb="FF00CC00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CC33"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FF00CC00"/>
+        <bgColor rgb="FF00CC33"/>
       </patternFill>
     </fill>
   </fills>
@@ -217,7 +229,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,18 +253,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,22 +275,25 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Untitled1" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00CC33"/>
+      <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -317,7 +331,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF66FF66"/>
+      <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -325,7 +339,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -342,16 +356,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,6 +1289,551 @@
       </c>
       <c r="I30" s="4" t="n">
         <f aca="false">I28*100000</f>
+        <v>-40463.6672247049</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>0.0120044816829252</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>0.152558189945</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>-0.0137818846721377</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>-0.0205396233995499</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>-0.0137819079000626</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>-0.0633109087448499</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>-0.0564613894828751</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>-0.0633109087448499</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>-0.0633109087448499</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>-0.0633109087448499</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>0.0289191389530751</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>0.00576395799200009</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>0.0289191389530751</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>0.0202253951186001</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>0.0289191389530751</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>-0.00913559413217495</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0.09765636168265</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>0.00248123137499996</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>0.00248123137499996</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>0.00248123137499996</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>-0.00510469515281242</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>-0.00589258853972496</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>-0.00510469515281242</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>0.00637622290493779</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>0.0300602910500374</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0.06366964780525</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>-0.0179367606699116</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>0.00580650598830042</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>0.0172739398504376</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>0.00580650598830042</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>-0.000303738749999831</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>-0.000505641013262274</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>-0.000303738749999831</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>0.0292941988334629</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>-0.000303738749999831</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>-0.0660723775557375</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>-0.0545773541521873</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>-0.0660723775557375</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>-0.0627954844512999</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>-0.0660723775557375</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>0.0119972894966628</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>0.0541013470171129</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>0.0142201487413999</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>0.0142201487413999</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>0.0119972894966628</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>-0.0194904622287377</v>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>0.0583873692714628</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>-0.0194904622287377</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>-0.0194904622287377</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>-0.0194904622287377</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>-0.101159168061762</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>-0.101159168061762</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>-0.101159168061762</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>-0.101159168061762</v>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>-0.101159168061762</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <f aca="false">AVERAGE(B34:B44)*4</f>
+        <v>-0.0538132315229678</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <f aca="false">AVERAGE(C34:C44)*4</f>
+        <v>0.0479761178140007</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <f aca="false">AVERAGE(D34:D44)*4</f>
+        <v>-0.0791986218575498</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <f aca="false">AVERAGE(E34:E44)*4</f>
+        <v>-0.0645180036590405</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <f aca="false">AVERAGE(F34:F44)*4</f>
+        <v>-0.0672196750465724</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="4" t="n">
+        <f aca="false">B47*100000</f>
+        <v>-5381.32315229678</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f aca="false">C47*100000</f>
+        <v>4797.61178140007</v>
+      </c>
+      <c r="D48" s="4" t="n">
+        <f aca="false">D47*100000</f>
+        <v>-7919.86218575498</v>
+      </c>
+      <c r="E48" s="4" t="n">
+        <f aca="false">E47*100000</f>
+        <v>-6451.80036590405</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <f aca="false">F47*100000</f>
+        <v>-6721.96750465724</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <f aca="false">STDEV(B34:B44)*SQRT(4)</f>
+        <v>0.0944113799405209</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <f aca="false">STDEV(C34:C44)*SQRT(4)</f>
+        <v>0.147450418795178</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <f aca="false">STDEV(D34:D44)*SQRT(4)</f>
+        <v>0.0799226813491694</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <f aca="false">STDEV(E34:E44)*SQRT(4)</f>
+        <v>0.0847097109316406</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <f aca="false">STDEV(F34:F44)*SQRT(4)</f>
+        <v>0.0848391544440517</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="4" t="n">
+        <f aca="false">B49*100000</f>
+        <v>9441.13799405209</v>
+      </c>
+      <c r="C50" s="4" t="n">
+        <f aca="false">C49*100000</f>
+        <v>14745.0418795178</v>
+      </c>
+      <c r="D50" s="4" t="n">
+        <f aca="false">D49*100000</f>
+        <v>7992.26813491694</v>
+      </c>
+      <c r="E50" s="4" t="n">
+        <f aca="false">E49*100000</f>
+        <v>8470.97109316406</v>
+      </c>
+      <c r="F50" s="4" t="n">
+        <f aca="false">F49*100000</f>
+        <v>8483.91544440517</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="4" t="n">
+        <f aca="false">B47/B49</f>
+        <v>-0.569986706654114</v>
+      </c>
+      <c r="C51" s="4" t="n">
+        <f aca="false">C47/C49</f>
+        <v>0.325371187182884</v>
+      </c>
+      <c r="D51" s="4" t="n">
+        <f aca="false">D47/D49</f>
+        <v>-0.990940500501273</v>
+      </c>
+      <c r="E51" s="4" t="n">
+        <f aca="false">E47/E49</f>
+        <v>-0.761636451706293</v>
+      </c>
+      <c r="F51" s="4" t="n">
+        <f aca="false">F47/F49</f>
+        <v>-0.792319012218601</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="4" t="n">
+        <f aca="false">B51*100000</f>
+        <v>-56998.6706654114</v>
+      </c>
+      <c r="C52" s="4" t="n">
+        <f aca="false">C51*100000</f>
+        <v>32537.1187182884</v>
+      </c>
+      <c r="D52" s="4" t="n">
+        <f aca="false">D51*100000</f>
+        <v>-99094.0500501273</v>
+      </c>
+      <c r="E52" s="4" t="n">
+        <f aca="false">E51*100000</f>
+        <v>-76163.6451706293</v>
+      </c>
+      <c r="F52" s="4" t="n">
+        <f aca="false">F51*100000</f>
+        <v>-79231.9012218601</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <f aca="false">COUNTIF(B34:B44,"&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <f aca="false">COUNTIF(C34:C44,"&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <f aca="false">COUNTIF(D34:D44,"&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <f aca="false">COUNTIF(E34:E44,"&gt;0")</f>
+        <v>6</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <f aca="false">COUNTIF(F34:F44,"&gt;0")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <f aca="false">COUNTIF(B34:B44,"&lt;=0")</f>
+        <v>7</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <f aca="false">COUNTIF(C34:C44,"&lt;=0")</f>
+        <v>6</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <f aca="false">COUNTIF(D34:D44,"&lt;=0")</f>
+        <v>7</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">COUNTIF(E34:E44,"&lt;=0")</f>
+        <v>5</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <f aca="false">COUNTIF(F34:F44,"&lt;=0")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="3" t="n">
+        <f aca="false">MAX(B34:B44)*4</f>
+        <v>0.254678591221</v>
+      </c>
+      <c r="C55" s="3" t="n">
+        <f aca="false">MAX(C34:C44)*4</f>
+        <v>0.610232759779999</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <f aca="false">MAX(D34:D44)*4</f>
+        <v>0.115676555812301</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <f aca="false">MAX(E34:E44)*4</f>
+        <v>0.117176795333852</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <f aca="false">MAX(F34:F44)*4</f>
+        <v>0.12024116420015</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="3" t="n">
+        <f aca="false">MIN(B34:B44)*4</f>
+        <v>-0.404636672247049</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <f aca="false">MIN(C34:C44)*4</f>
+        <v>-0.404636672247049</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <f aca="false">MIN(D34:D44)*4</f>
+        <v>-0.404636672247049</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <f aca="false">MIN(E34:E44)*4</f>
+        <v>-0.404636672247049</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <f aca="false">MIN(F34:F44)*4</f>
+        <v>-0.404636672247049</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="4" t="n">
+        <f aca="false">B55*100000</f>
+        <v>25467.8591221</v>
+      </c>
+      <c r="C57" s="4" t="n">
+        <f aca="false">C55*100000</f>
+        <v>61023.2759779999</v>
+      </c>
+      <c r="D57" s="4" t="n">
+        <f aca="false">D55*100000</f>
+        <v>11567.6555812301</v>
+      </c>
+      <c r="E57" s="4" t="n">
+        <f aca="false">E55*100000</f>
+        <v>11717.6795333852</v>
+      </c>
+      <c r="F57" s="4" t="n">
+        <f aca="false">F55*100000</f>
+        <v>12024.116420015</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="4" t="n">
+        <f aca="false">B56*100000</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="C58" s="4" t="n">
+        <f aca="false">C56*100000</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="D58" s="4" t="n">
+        <f aca="false">D56*100000</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="E58" s="4" t="n">
+        <f aca="false">E56*100000</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="F58" s="4" t="n">
+        <f aca="false">F56*100000</f>
         <v>-40463.6672247049</v>
       </c>
     </row>
@@ -1293,29 +1853,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1781,7 +2342,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +2384,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">B19/100000</f>
@@ -1897,7 +2458,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">B21/100000</f>
@@ -2082,7 +2643,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>8313.59</v>
@@ -2090,17 +2651,462 @@
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">B28/100000</f>
         <v>0.0831359</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>6468.17894779252</v>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>20523.549774</v>
+      </c>
+      <c r="D32" s="4" t="n">
+        <v>3889.54231228624</v>
+      </c>
+      <c r="E32" s="4" t="n">
+        <v>3213.76843954502</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <v>3889.53998949375</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>-6331.09087448499</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>-5646.13894828751</v>
+      </c>
+      <c r="D33" s="4" t="n">
+        <v>-6331.09087448499</v>
+      </c>
+      <c r="E33" s="4" t="n">
+        <v>-6331.09087448499</v>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>-6331.09087448499</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>3740.25753330753</v>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>1424.73943720003</v>
+      </c>
+      <c r="D34" s="4" t="n">
+        <v>3740.25753330753</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>2870.88314986003</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>3740.25753330753</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>4046.5911927825</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>14725.786774265</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <v>5208.27374349999</v>
+      </c>
+      <c r="E35" s="4" t="n">
+        <v>5208.27374349999</v>
+      </c>
+      <c r="F35" s="4" t="n">
+        <v>5208.27374349999</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>3751.49128193752</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>3672.70194324627</v>
+      </c>
+      <c r="D36" s="4" t="n">
+        <v>3751.49128193752</v>
+      </c>
+      <c r="E36" s="4" t="n">
+        <v>4899.58308771254</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>7267.98990222251</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>10412.884673885</v>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>2252.24382636884</v>
+      </c>
+      <c r="D37" s="4" t="n">
+        <v>4626.57049219004</v>
+      </c>
+      <c r="E37" s="4" t="n">
+        <v>5773.31387840376</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>4626.57049219004</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>3895.51822738752</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <v>3875.32800106127</v>
+      </c>
+      <c r="D38" s="4" t="n">
+        <v>3895.51822738752</v>
+      </c>
+      <c r="E38" s="4" t="n">
+        <v>6855.31198573379</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>3895.51822738752</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>-6607.23775557375</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>-5457.73541521873</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <v>-6607.23775557375</v>
+      </c>
+      <c r="E39" s="4" t="n">
+        <v>-6279.54844512999</v>
+      </c>
+      <c r="F39" s="4" t="n">
+        <v>-6607.23775557375</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>167.925349666276</v>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>4378.33110171129</v>
+      </c>
+      <c r="D40" s="4" t="n">
+        <v>390.211274139995</v>
+      </c>
+      <c r="E40" s="4" t="n">
+        <v>390.211274139995</v>
+      </c>
+      <c r="F40" s="4" t="n">
+        <v>167.925349666276</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>161.483905247506</v>
+      </c>
+      <c r="C41" s="4" t="n">
+        <v>7949.26705526755</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <v>161.483905247506</v>
+      </c>
+      <c r="E41" s="4" t="n">
+        <v>161.483905247506</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <v>161.483905247506</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="4" t="n">
+        <v>-10115.9168061762</v>
+      </c>
+      <c r="C42" s="4" t="n">
+        <v>-10115.9168061762</v>
+      </c>
+      <c r="D42" s="4" t="n">
+        <v>-10115.9168061762</v>
+      </c>
+      <c r="E42" s="4" t="n">
+        <v>-10115.9168061762</v>
+      </c>
+      <c r="F42" s="4" t="n">
+        <v>-10115.9168061762</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <f aca="false">AVERAGE(B32:B42)*4</f>
+        <v>3487.30388209869</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <f aca="false">AVERAGE(C32:C42)*4</f>
+        <v>13666.2388157955</v>
+      </c>
+      <c r="D45" s="3" t="n">
+        <f aca="false">AVERAGE(D32:D42)*4</f>
+        <v>948.764848640504</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <f aca="false">AVERAGE(E32:E42)*4</f>
+        <v>2416.82666849143</v>
+      </c>
+      <c r="F45" s="3" t="n">
+        <f aca="false">AVERAGE(F32:F42)*4</f>
+        <v>2146.65952973824</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <f aca="false">B45/100000</f>
+        <v>0.0348730388209869</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <f aca="false">C45/100000</f>
+        <v>0.136662388157955</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <f aca="false">D45/100000</f>
+        <v>0.00948764848640504</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <f aca="false">E45/100000</f>
+        <v>0.0241682666849143</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <f aca="false">F45/100000</f>
+        <v>0.0214665952973824</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <f aca="false">STDEV(B32:B42)*SQRT(4)</f>
+        <v>12452.1828993922</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <f aca="false">STDEV(C32:C42)*SQRT(4)</f>
+        <v>17794.7269065245</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <f aca="false">STDEV(D32:D42)*SQRT(4)</f>
+        <v>10817.1649811992</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <f aca="false">STDEV(E32:E42)*SQRT(4)</f>
+        <v>11454.9307360085</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <f aca="false">STDEV(F32:F42)*SQRT(4)</f>
+        <v>11464.8036563724</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <f aca="false">B47/100000</f>
+        <v>0.124521828993922</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <f aca="false">C47/100000</f>
+        <v>0.177947269065245</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <f aca="false">D47/100000</f>
+        <v>0.108171649811992</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <f aca="false">E47/100000</f>
+        <v>0.114549307360085</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <f aca="false">F47/100000</f>
+        <v>0.114648036563724</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <f aca="false">COUNTIF(B32:B42,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <f aca="false">COUNTIF(C32:C42,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">COUNTIF(D32:D42,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">COUNTIF(E32:E42,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <f aca="false">COUNTIF(F32:F42,"&gt;0")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <f aca="false">COUNTIF(B32:B42,"&lt;=0")</f>
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <f aca="false">COUNTIF(C32:C42,"&lt;=0")</f>
+        <v>3</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">COUNTIF(D32:D42,"&lt;=0")</f>
+        <v>3</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">COUNTIF(E32:E42,"&lt;=0")</f>
+        <v>3</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <f aca="false">COUNTIF(F32:F42,"&lt;=0")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <f aca="false">MAX(B32:B42)*4</f>
+        <v>41651.53869554</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <f aca="false">MAX(C32:C42)*4</f>
+        <v>82094.1990959999</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <f aca="false">MAX(D32:D42)*4</f>
+        <v>20833.094974</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <f aca="false">MAX(E32:E42)*4</f>
+        <v>27421.2479429352</v>
+      </c>
+      <c r="F51" s="3" t="n">
+        <f aca="false">MAX(F32:F42)*4</f>
+        <v>29071.95960889</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="3" t="n">
+        <f aca="false">MIN(B32:B42)*4</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <f aca="false">MIN(C32:C42)*4</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <f aca="false">MIN(D32:D42)*4</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <f aca="false">MIN(E32:E42)*4</f>
+        <v>-40463.6672247049</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <f aca="false">MIN(F32:F42)*4</f>
+        <v>-40463.6672247049</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Agrega nuevos resultados para mid h=1 corrigiendo problema con etiquetado
</commit_message>
<xml_diff>
--- a/experimentos/comparacion_experimentos.xlsx
+++ b/experimentos/comparacion_experimentos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Exceso_sobre_BH_90_dicc1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Exceso_sobre_BH_90_dicc2_open" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Ganancia_Total_90_dicc2_open" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="naftrac" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="presentacion" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="1750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="1758">
   <si>
     <t>Periodo Prueba</t>
   </si>
@@ -5274,6 +5275,30 @@
   </si>
   <si>
     <t>2019-01-25</t>
+  </si>
+  <si>
+    <t>AQ TI Top 5</t>
+  </si>
+  <si>
+    <t>AQ TI</t>
+  </si>
+  <si>
+    <t>CN2 TI Top 5</t>
+  </si>
+  <si>
+    <t>CN2 TI</t>
+  </si>
+  <si>
+    <t>AQ EA Top 5</t>
+  </si>
+  <si>
+    <t>AQ EA</t>
+  </si>
+  <si>
+    <t>CN2 EA Top 5</t>
+  </si>
+  <si>
+    <t>CN2 EA</t>
   </si>
 </sst>
 </file>
@@ -5412,20 +5437,20 @@
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="12.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5462,28 +5487,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0130755506501756</v>
+        <v>0.0674408240963877</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.0183587547974131</v>
+        <v>0.0421884537483253</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.1104795345017</v>
+        <v>0.00956221745020014</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-0.00256234387032406</v>
+        <v>0.00053727644224999</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.0385772902000003</v>
+        <v>-0.0487195300324247</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.0385772902000003</v>
+        <v>0.0432980349925627</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-0.0134815076331996</v>
+        <v>0.0344732430103754</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>-0.0134815076331996</v>
+        <v>0.0344732430103754</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5491,28 +5516,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.0197351509110746</v>
+        <v>0.00486948659140052</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.0189496725927628</v>
+        <v>-0.0626917068755992</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-3.49243041122271E-005</v>
+        <v>-0.0186213428998615</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-0.00128990138396223</v>
+        <v>-0.00330300784578674</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>-0.000575639994075172</v>
+        <v>-0.0293633440451</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>-0.0286238770041365</v>
+        <v>-0.0143326944941374</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>-0.00407200686089959</v>
+        <v>-0.00909813114954972</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>-0.0168078935691373</v>
+        <v>-0.000777122117086804</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5520,28 +5545,28 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>-0.0411142343933249</v>
+        <v>-0.0311127349387497</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>-0.00944771824717514</v>
+        <v>-0.0069965829215751</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>-0.0121465246739997</v>
+        <v>-0.0311127349387497</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-0.00532453413178743</v>
+        <v>-0.00954661340046256</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>-0.00361464853747515</v>
+        <v>-0.0311127349387497</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>-0.00636665159036251</v>
+        <v>-0.0076662036945748</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>-0.0298754019395374</v>
+        <v>-0.00387809530068659</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>-0.00700997545224977</v>
+        <v>-0.00865996241864972</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5549,28 +5574,28 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>-0.0163325042736123</v>
+        <v>-0.00393804061753751</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>-0.0648688113688494</v>
+        <v>-0.0367728109988624</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.00581001520157513</v>
+        <v>-0.0247752367477495</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.0413859647276249</v>
+        <v>-0.000921975776911513</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>-0.0557496185377249</v>
+        <v>0.00735312925421287</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.0389137985281752</v>
+        <v>0.0026903729321001</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>-0.00882145639954963</v>
+        <v>0.00439253568003754</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>-0.0609575869349243</v>
+        <v>-0.0646235879025742</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5578,28 +5603,28 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>-0.0195393921252744</v>
+        <v>0.0687758469737625</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.037617562126425</v>
+        <v>0.0375151514829373</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.0262957760811129</v>
+        <v>0.0295716773670876</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.0308428512317876</v>
+        <v>-0.0320475778858619</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>-0.018497421839587</v>
+        <v>-0.00593444241803737</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>-0.0307319450757372</v>
+        <v>0.0390514666001125</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.0226314733809501</v>
+        <v>0.0366985267924627</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>-0.0148814206365621</v>
+        <v>-0.0145141299341249</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5607,28 +5632,28 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.0226993843243373</v>
+        <v>0.0229511796826502</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.0229511796826502</v>
+        <v>0.00603308534509995</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.0123819845023875</v>
+        <v>0.0116570733021877</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.0147632522795873</v>
+        <v>0.0184939718880123</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>-0.0168542424188622</v>
+        <v>-0.0334935323554123</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.0311755049271872</v>
+        <v>0.0184939718880123</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0.0175957570545001</v>
+        <v>0.0116570733021877</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>-0.0596634151475245</v>
+        <v>-0.0371686491606126</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5636,28 +5661,28 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>-0.0130447476648873</v>
+        <v>0.0280683615787007</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>-0.0514759660308498</v>
+        <v>-0.0127312296457121</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>-0.0161234137053123</v>
+        <v>-0.034354516490812</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.00323862054932525</v>
+        <v>-0.00288543721433729</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>-0.0647153162008995</v>
+        <v>-0.000807669985749632</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.017745331078238</v>
+        <v>0.00044084468641295</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.0308765597529252</v>
+        <v>-0.034354516490812</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>-0.00842955851154933</v>
+        <v>0.012829299567925</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5665,28 +5690,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="2" t="n">
+        <v>-0.0398470373906627</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>-0.0013605933535876</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.0415896942977121</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <v>0.00245818912499975</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>-0.0398581419555373</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>-0.0394984512397247</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0.00595659026339981</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.00245818912499975</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.0389483264813249</v>
+        <v>0.00456525519765007</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>-0.0398470373906627</v>
+        <v>0.0415896942977121</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.00595659026339981</v>
+        <v>0.0400345735705372</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5694,28 +5719,28 @@
         <v>17</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0460202754383499</v>
+        <v>-0.0318037943075251</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.00538143471494992</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.00886941952847489</v>
+        <v>0.0460202754383499</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>-0.0380618739531249</v>
+        <v>0.00538143471494992</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-0.0269047527396497</v>
+        <v>0.00489168507610007</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0.00538143471494992</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>-0.000433804993274813</v>
+        <v>0.0460202754383499</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.00692232271265027</v>
+        <v>0.00956869260584983</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5723,28 +5748,28 @@
         <v>18</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.021026032577988</v>
+        <v>0.0165024344875503</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>-0.0071141169717749</v>
+        <v>0.0516417621938504</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>5.56510000001426E-005</v>
+        <v>0.0144289757688</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.0114823705375505</v>
+        <v>0.0138708093615002</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>-0.0011790757599749</v>
+        <v>0.0144289757688</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>-0.0011790757599749</v>
+        <v>0.0158162429319754</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.00379699371520013</v>
+        <v>0.0144289757688</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.0115933250922006</v>
+        <v>0.019605854820863</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5752,28 +5777,28 @@
         <v>19</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.00151042481657528</v>
+        <v>0.00108595610096298</v>
       </c>
       <c r="C12" s="2" t="n">
+        <v>0.00181431243104981</v>
+      </c>
+      <c r="D12" s="2" t="n">
         <v>0.00136728886997508</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>0.0028476146248503</v>
-      </c>
       <c r="E12" s="2" t="n">
+        <v>0.00412571868613778</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.00412571868613778</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0.00352551817352533</v>
+      </c>
+      <c r="H12" s="2" t="n">
         <v>0.00136728886997508</v>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>0.00352551817352533</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>0.000867427846000045</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>0.000940047124450415</v>
-      </c>
       <c r="I12" s="2" t="n">
-        <v>0.0028476146248503</v>
+        <v>0.00412571868613778</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,28 +5806,28 @@
         <v>20</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.00436754369382479</v>
+        <v>0.0211571536073625</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>-0.00596149628737504</v>
+        <v>0.00350330640547474</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.00699726460807519</v>
+        <v>0.023379501677175</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.0121319214911997</v>
+        <v>-0.0103490157533</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.00611456519382485</v>
+        <v>0.0211571536073625</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0.00350330640547474</v>
+        <v>-0.0200554688858997</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>0.00146482485616233</v>
+        <v>0.023379501677175</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>-0.0015945620232249</v>
+        <v>-0.00406498970640042</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5810,28 +5835,28 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0.0393071278343624</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.0236528200416504</v>
+        <v>-0.0141694233531998</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>-0.0243195564293249</v>
+        <v>0.00086796792697541</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.0125369332084</v>
+        <v>-0.0346201215986999</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.0111975890294376</v>
+        <v>0.000393698970000189</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>0.0223089931613132</v>
+        <v>-0.0599513281816746</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>-0.0303095106845125</v>
+        <v>0.00086796792697541</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>-0.0257595885813</v>
+        <v>0.00413940004841273</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5839,28 +5864,28 @@
         <v>22</v>
       </c>
       <c r="B15" s="2" t="n">
+        <v>0.051668476902525</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>-0.0267844313185747</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>-0.0285992099473499</v>
+      </c>
+      <c r="E15" s="2" t="n">
         <v>0.0108053295934499</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>-0.0264043090103502</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>-0.00825674400117483</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>-0.0290439301818751</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0.0108053295934499</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>-0.00556753151035018</v>
+        <v>0.01343807574105</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>-0.0369693785768999</v>
+        <v>-0.0285992099473499</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>-0.0253291801634875</v>
+        <v>0.0108053295934499</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5868,28 +5893,28 @@
         <v>23</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0.080828294931575</v>
+        <v>0.0811824312935124</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.0238859274291004</v>
+        <v>0.0323678445289004</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.0552423315891628</v>
+        <v>-0.020559566529962</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-0.0312093447930746</v>
+        <v>-0.0071593970301622</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0.00734840989392539</v>
+        <v>0.00347515742837491</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>-0.0283247976740495</v>
+        <v>-0.0185222163983624</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0.0383337214950004</v>
+        <v>-0.020559566529962</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.0841388288723263</v>
+        <v>0.00282154268576286</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5913,35 +5938,35 @@
       </c>
       <c r="B19" s="2" t="n">
         <f aca="false">AVERAGE(B2:B16)*4</f>
-        <v>0.0352885662979905</v>
+        <v>0.0685334784160906</v>
       </c>
       <c r="C19" s="2" t="n">
         <f aca="false">AVERAGE(C2:C16)*4</f>
-        <v>-0.014124245231196</v>
+        <v>0.00505028596892716</v>
       </c>
       <c r="D19" s="2" t="n">
         <f aca="false">AVERAGE(D2:D16)*4</f>
-        <v>0.0342933272756508</v>
+        <v>0.00544588387839421</v>
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">AVERAGE(E2:E16)*4</f>
-        <v>0.00699036395858718</v>
+        <v>-0.0120427777851259</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">AVERAGE(F2:F16)*4</f>
-        <v>-0.0288170199517561</v>
+        <v>-0.0214245910042762</v>
       </c>
       <c r="G19" s="2" t="n">
         <f aca="false">AVERAGE(G2:G16)*4</f>
-        <v>0.0257673425941474</v>
+        <v>0.00697954832098731</v>
       </c>
       <c r="H19" s="2" t="n">
         <f aca="false">AVERAGE(H2:H16)*4</f>
-        <v>-0.0128455272264926</v>
+        <v>0.0315694835588508</v>
       </c>
       <c r="I19" s="2" t="n">
         <f aca="false">AVERAGE(I2:I16)*4</f>
-        <v>-0.0326549352233952</v>
+        <v>0.00229205689329734</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5950,35 +5975,35 @@
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">B19*100000</f>
-        <v>3528.85662979905</v>
+        <v>6853.34784160906</v>
       </c>
       <c r="C20" s="3" t="n">
         <f aca="false">C19*100000</f>
-        <v>-1412.4245231196</v>
+        <v>505.028596892716</v>
       </c>
       <c r="D20" s="3" t="n">
         <f aca="false">D19*100000</f>
-        <v>3429.33272756508</v>
+        <v>544.588387839421</v>
       </c>
       <c r="E20" s="3" t="n">
         <f aca="false">E19*100000</f>
-        <v>699.036395858718</v>
+        <v>-1204.27777851259</v>
       </c>
       <c r="F20" s="3" t="n">
         <f aca="false">F19*100000</f>
-        <v>-2881.70199517561</v>
+        <v>-2142.45910042762</v>
       </c>
       <c r="G20" s="3" t="n">
         <f aca="false">G19*100000</f>
-        <v>2576.73425941474</v>
+        <v>697.954832098731</v>
       </c>
       <c r="H20" s="3" t="n">
         <f aca="false">H19*100000</f>
-        <v>-1284.55272264926</v>
+        <v>3156.94835588508</v>
       </c>
       <c r="I20" s="3" t="n">
         <f aca="false">I19*100000</f>
-        <v>-3265.49352233952</v>
+        <v>229.205689329734</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5987,35 +6012,35 @@
       </c>
       <c r="B21" s="2" t="n">
         <f aca="false">STDEV(B2:B16)*SQRT(4)</f>
-        <v>0.0614113014201638</v>
+        <v>0.0751712894512434</v>
       </c>
       <c r="C21" s="2" t="n">
         <f aca="false">STDEV(C2:C16)*SQRT(4)</f>
-        <v>0.0607824568026915</v>
+        <v>0.0618116225285485</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">STDEV(D2:D16)*SQRT(4)</f>
-        <v>0.0713070553331863</v>
+        <v>0.0535281062543234</v>
       </c>
       <c r="E21" s="2" t="n">
         <f aca="false">STDEV(E2:E16)*SQRT(4)</f>
-        <v>0.0435008165947927</v>
+        <v>0.029581425980797</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">STDEV(F2:F16)*SQRT(4)</f>
-        <v>0.052705796186914</v>
+        <v>0.0407677443192299</v>
       </c>
       <c r="G21" s="2" t="n">
         <f aca="false">STDEV(G2:G16)*SQRT(4)</f>
-        <v>0.0488802758443385</v>
+        <v>0.0501430691626776</v>
       </c>
       <c r="H21" s="2" t="n">
         <f aca="false">STDEV(H2:H16)*SQRT(4)</f>
-        <v>0.0482536404327175</v>
+        <v>0.050369128922219</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">STDEV(I2:I16)*SQRT(4)</f>
-        <v>0.0669641375939089</v>
+        <v>0.0519509624355256</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6024,35 +6049,35 @@
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">B21*100000</f>
-        <v>6141.13014201638</v>
+        <v>7517.12894512434</v>
       </c>
       <c r="C22" s="3" t="n">
         <f aca="false">C21*100000</f>
-        <v>6078.24568026915</v>
+        <v>6181.16225285485</v>
       </c>
       <c r="D22" s="3" t="n">
         <f aca="false">D21*100000</f>
-        <v>7130.70553331863</v>
+        <v>5352.81062543234</v>
       </c>
       <c r="E22" s="3" t="n">
         <f aca="false">E21*100000</f>
-        <v>4350.08165947927</v>
+        <v>2958.1425980797</v>
       </c>
       <c r="F22" s="3" t="n">
         <f aca="false">F21*100000</f>
-        <v>5270.5796186914</v>
+        <v>4076.77443192299</v>
       </c>
       <c r="G22" s="3" t="n">
         <f aca="false">G21*100000</f>
-        <v>4888.02758443385</v>
+        <v>5014.30691626776</v>
       </c>
       <c r="H22" s="3" t="n">
         <f aca="false">H21*100000</f>
-        <v>4825.36404327175</v>
+        <v>5036.9128922219</v>
       </c>
       <c r="I22" s="3" t="n">
         <f aca="false">I21*100000</f>
-        <v>6696.41375939089</v>
+        <v>5195.09624355256</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6061,35 +6086,35 @@
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">B19/B21</f>
-        <v>0.574626583086934</v>
+        <v>0.911697523301656</v>
       </c>
       <c r="C23" s="3" t="n">
         <f aca="false">C19/C21</f>
-        <v>-0.232373713965615</v>
+        <v>0.0817044717859432</v>
       </c>
       <c r="D23" s="3" t="n">
         <f aca="false">D19/D21</f>
-        <v>0.480924743216688</v>
+        <v>0.101738773505636</v>
       </c>
       <c r="E23" s="3" t="n">
         <f aca="false">E19/E21</f>
-        <v>0.160695005422587</v>
+        <v>-0.407106060165714</v>
       </c>
       <c r="F23" s="3" t="n">
         <f aca="false">F19/F21</f>
-        <v>-0.546752388476601</v>
+        <v>-0.525527996754296</v>
       </c>
       <c r="G23" s="3" t="n">
         <f aca="false">G19/G21</f>
-        <v>0.527152151845555</v>
+        <v>0.139192682808142</v>
       </c>
       <c r="H23" s="3" t="n">
         <f aca="false">H19/H21</f>
-        <v>-0.266208458290392</v>
+        <v>0.626762547504068</v>
       </c>
       <c r="I23" s="3" t="n">
         <f aca="false">I19/I21</f>
-        <v>-0.487648111313324</v>
+        <v>0.0441196233109623</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6098,35 +6123,35 @@
       </c>
       <c r="B24" s="3" t="n">
         <f aca="false">B23*100000</f>
-        <v>57462.6583086934</v>
+        <v>91169.7523301656</v>
       </c>
       <c r="C24" s="3" t="n">
         <f aca="false">C23*100000</f>
-        <v>-23237.3713965615</v>
+        <v>8170.44717859432</v>
       </c>
       <c r="D24" s="3" t="n">
         <f aca="false">D23*100000</f>
-        <v>48092.4743216689</v>
+        <v>10173.8773505636</v>
       </c>
       <c r="E24" s="3" t="n">
         <f aca="false">E23*100000</f>
-        <v>16069.5005422587</v>
+        <v>-40710.6060165714</v>
       </c>
       <c r="F24" s="3" t="n">
         <f aca="false">F23*100000</f>
-        <v>-54675.2388476601</v>
+        <v>-52552.7996754296</v>
       </c>
       <c r="G24" s="3" t="n">
         <f aca="false">G23*100000</f>
-        <v>52715.2151845555</v>
+        <v>13919.2682808142</v>
       </c>
       <c r="H24" s="3" t="n">
         <f aca="false">H23*100000</f>
-        <v>-26620.8458290392</v>
+        <v>62676.2547504068</v>
       </c>
       <c r="I24" s="3" t="n">
         <f aca="false">I23*100000</f>
-        <v>-48764.8111313324</v>
+        <v>4411.96233109623</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6147,23 +6172,23 @@
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">COUNTIF(E2:E16,"&gt;0")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F25" s="0" t="n">
         <f aca="false">COUNTIF(F2:F16,"&gt;0")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">COUNTIF(G2:G16,"&gt;0")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H25" s="0" t="n">
         <f aca="false">COUNTIF(H2:H16,"&gt;0")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I25" s="0" t="n">
         <f aca="false">COUNTIF(I2:I16,"&gt;0")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6184,23 +6209,23 @@
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">COUNTIF(E2:E16,"&lt;=0")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">COUNTIF(F2:F16,"&lt;=0")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">COUNTIF(G2:G16,"&lt;=0")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">COUNTIF(H2:H16,"&lt;=0")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">COUNTIF(I2:I16,"&lt;=0")</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6209,35 +6234,35 @@
       </c>
       <c r="B27" s="2" t="n">
         <f aca="false">MAX(B2:B16)*4</f>
-        <v>0.3233131797263</v>
+        <v>0.324729725174049</v>
       </c>
       <c r="C27" s="2" t="n">
         <f aca="false">MAX(C2:C16)*4</f>
-        <v>0.1504702485057</v>
+        <v>0.206567048775402</v>
       </c>
       <c r="D27" s="2" t="n">
         <f aca="false">MAX(D2:D16)*4</f>
-        <v>0.441918138006802</v>
+        <v>0.1840811017534</v>
       </c>
       <c r="E27" s="2" t="n">
         <f aca="false">MAX(E2:E16)*4</f>
-        <v>0.1655438589105</v>
+        <v>0.0739758875520491</v>
       </c>
       <c r="F27" s="2" t="n">
         <f aca="false">MAX(F2:F16)*4</f>
-        <v>0.154309160800001</v>
+        <v>0.0846286144294501</v>
       </c>
       <c r="G27" s="2" t="n">
         <f aca="false">MAX(G2:G16)*4</f>
-        <v>0.1557933059253</v>
+        <v>0.173192139970251</v>
       </c>
       <c r="H27" s="2" t="n">
         <f aca="false">MAX(H2:H16)*4</f>
-        <v>0.153334885980002</v>
+        <v>0.1840811017534</v>
       </c>
       <c r="I27" s="2" t="n">
         <f aca="false">MAX(I2:I16)*4</f>
-        <v>0.336555315489305</v>
+        <v>0.160138294282149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6246,35 +6271,35 @@
       </c>
       <c r="B28" s="2" t="n">
         <f aca="false">MIN(B2:B16)*4</f>
-        <v>-0.1644569375733</v>
+        <v>-0.159388149562651</v>
       </c>
       <c r="C28" s="2" t="n">
         <f aca="false">MIN(C2:C16)*4</f>
-        <v>-0.259475245475398</v>
+        <v>-0.250766827502397</v>
       </c>
       <c r="D28" s="2" t="n">
         <f aca="false">MIN(D2:D16)*4</f>
-        <v>-0.157993804958899</v>
+        <v>-0.137418065963248</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">MIN(E2:E16)*4</f>
-        <v>-0.152247495812499</v>
+        <v>-0.138480486394799</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">MIN(F2:F16)*4</f>
-        <v>-0.258861264803598</v>
+        <v>-0.194878120129699</v>
       </c>
       <c r="G28" s="2" t="n">
         <f aca="false">MIN(G2:G16)*4</f>
-        <v>-0.122927780302949</v>
+        <v>-0.239805312726698</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">MIN(H2:H16)*4</f>
-        <v>-0.159388149562651</v>
+        <v>-0.137418065963248</v>
       </c>
       <c r="I28" s="2" t="n">
         <f aca="false">MIN(I2:I16)*4</f>
-        <v>-0.243830347739697</v>
+        <v>-0.258494351610297</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6283,35 +6308,35 @@
       </c>
       <c r="B29" s="3" t="n">
         <f aca="false">B27*100000</f>
-        <v>32331.31797263</v>
+        <v>32472.9725174049</v>
       </c>
       <c r="C29" s="3" t="n">
         <f aca="false">C27*100000</f>
-        <v>15047.02485057</v>
+        <v>20656.7048775402</v>
       </c>
       <c r="D29" s="3" t="n">
         <f aca="false">D27*100000</f>
-        <v>44191.8138006802</v>
+        <v>18408.11017534</v>
       </c>
       <c r="E29" s="3" t="n">
         <f aca="false">E27*100000</f>
-        <v>16554.38589105</v>
+        <v>7397.58875520491</v>
       </c>
       <c r="F29" s="3" t="n">
         <f aca="false">F27*100000</f>
-        <v>15430.9160800001</v>
+        <v>8462.86144294501</v>
       </c>
       <c r="G29" s="3" t="n">
         <f aca="false">G27*100000</f>
-        <v>15579.33059253</v>
+        <v>17319.2139970251</v>
       </c>
       <c r="H29" s="3" t="n">
         <f aca="false">H27*100000</f>
-        <v>15333.4885980002</v>
+        <v>18408.11017534</v>
       </c>
       <c r="I29" s="3" t="n">
         <f aca="false">I27*100000</f>
-        <v>33655.5315489305</v>
+        <v>16013.8294282149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6320,35 +6345,35 @@
       </c>
       <c r="B30" s="3" t="n">
         <f aca="false">B28*100000</f>
-        <v>-16445.69375733</v>
+        <v>-15938.8149562651</v>
       </c>
       <c r="C30" s="3" t="n">
         <f aca="false">C28*100000</f>
-        <v>-25947.5245475398</v>
+        <v>-25076.6827502397</v>
       </c>
       <c r="D30" s="3" t="n">
         <f aca="false">D28*100000</f>
-        <v>-15799.3804958899</v>
+        <v>-13741.8065963248</v>
       </c>
       <c r="E30" s="3" t="n">
         <f aca="false">E28*100000</f>
-        <v>-15224.7495812499</v>
+        <v>-13848.0486394799</v>
       </c>
       <c r="F30" s="3" t="n">
         <f aca="false">F28*100000</f>
-        <v>-25886.1264803598</v>
+        <v>-19487.8120129699</v>
       </c>
       <c r="G30" s="3" t="n">
         <f aca="false">G28*100000</f>
-        <v>-12292.7780302949</v>
+        <v>-23980.5312726698</v>
       </c>
       <c r="H30" s="3" t="n">
         <f aca="false">H28*100000</f>
-        <v>-15938.8149562651</v>
+        <v>-13741.8065963248</v>
       </c>
       <c r="I30" s="3" t="n">
         <f aca="false">I28*100000</f>
-        <v>-24383.0347739697</v>
+        <v>-25849.4351610297</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6689,21 +6714,21 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6740,28 +6765,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>1307.55506501756</v>
+        <v>6744.08240963877</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>1835.87547974131</v>
+        <v>4218.84537483253</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>11047.95345017</v>
+        <v>956.221745020014</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>-256.234387032406</v>
+        <v>53.727644224999</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>3857.72902000003</v>
+        <v>-4871.95300324247</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>3857.72902000003</v>
+        <v>4329.80349925627</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>-1348.15076331996</v>
+        <v>3447.32430103754</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>-1348.15076331996</v>
+        <v>3447.32430103754</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6769,28 +6794,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>-5406.56813019745</v>
+        <v>-2946.10437994994</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>-1538.08577981371</v>
+        <v>-9702.22372664992</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>-3436.54546950122</v>
+        <v>-5295.18732907615</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>-3562.04317748622</v>
+        <v>-3763.35382366867</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>-3490.61703849751</v>
+        <v>-6369.38744359999</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>-6295.44073950364</v>
+        <v>-4866.32248850374</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>-3840.25372517995</v>
+        <v>-4342.86615404497</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>-5113.84239600372</v>
+        <v>-3510.76525079868</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6798,28 +6823,28 @@
         <v>11</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>4902.75629500503</v>
+        <v>5902.90624046255</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>8069.40790962001</v>
+        <v>8314.52144218001</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>7799.52726693756</v>
+        <v>5902.90624046255</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>8481.72632115878</v>
+        <v>8059.51839429127</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>8652.71488059001</v>
+        <v>5902.90624046255</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>8377.51457530127</v>
+        <v>8247.55936488004</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>6026.63954038378</v>
+        <v>8626.37020426886</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>8313.18218911254</v>
+        <v>8148.18349247255</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6827,28 +6852,28 @@
         <v>12</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>-5308.97116336123</v>
+        <v>-4069.52479775375</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>-10162.6018728849</v>
+        <v>-7353.00183588624</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>-3094.71921584249</v>
+        <v>-6153.24441077495</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>462.875736762491</v>
+        <v>-3767.91831369115</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>-9250.6825897725</v>
+        <v>-2940.40781057872</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>215.659116817513</v>
+        <v>-3406.68344278999</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>-4557.86637595497</v>
+        <v>-3236.46716799625</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>-9771.47942949244</v>
+        <v>-10138.0795262574</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6856,28 +6881,28 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>3313.79272836882</v>
+        <v>12145.3166382725</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>9029.48815353877</v>
+        <v>9019.24708919</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>7897.30954900756</v>
+        <v>8224.89967760503</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>8352.01706407502</v>
+        <v>2062.97415231007</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>3417.98975693757</v>
+        <v>4674.28769909253</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>2194.53743332254</v>
+        <v>9172.87860090752</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>7530.87927899128</v>
+        <v>8937.58462014254</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>3779.58987724005</v>
+        <v>3816.31894748378</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6885,28 +6910,28 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>-3926.6462438125</v>
+        <v>-3901.46670798122</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>-3901.46670798122</v>
+        <v>-5593.27614173624</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>-4958.38622600748</v>
+        <v>-5030.87734602746</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>-4720.2594482875</v>
+        <v>-4347.187487445</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>-7882.00891813245</v>
+        <v>-9545.93791178746</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>-3079.03418352751</v>
+        <v>-4347.187487445</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>-4437.00897079622</v>
+        <v>-5030.87734602746</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>-12162.9261909987</v>
+        <v>-9913.44959230749</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6914,28 +6939,28 @@
         <v>15</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>-420.136527413706</v>
+        <v>3691.17439694508</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>-4263.25836400996</v>
+        <v>-388.784725496194</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>-728.003131456212</v>
+        <v>-2551.11341000618</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>1208.20029400754</v>
+        <v>595.79451764129</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>-5587.19338101493</v>
+        <v>803.571240500056</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>2658.87134689882</v>
+        <v>928.422707716314</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>3971.99421436754</v>
+        <v>-2551.11341000618</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>41.3823879200859</v>
+        <v>2167.26819586752</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6943,28 +6968,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>3848.64440370751</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>8143.67316883748</v>
+      </c>
+      <c r="E9" s="5" t="n">
         <v>4230.52265156625</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>-1.11045648745201</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>34.8586150938024</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>4580.36276540625</v>
       </c>
       <c r="F9" s="5" t="n">
         <v>4230.52265156625</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>7879.53638719876</v>
+        <v>4441.22925883128</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>0</v>
+        <v>8143.67316883748</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>4580.36276540625</v>
+        <v>7988.16109611999</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6972,28 +6997,28 @@
         <v>17</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>7782.4069745875</v>
+        <v>0</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>3718.5229022475</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>4067.3213836</v>
+        <v>7782.4069745875</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>-625.807964559977</v>
+        <v>3718.5229022475</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>489.904156787535</v>
+        <v>3669.54793836252</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>3718.5229022475</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>3136.99893142503</v>
+        <v>7782.4069745875</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>3872.61170201754</v>
+        <v>4137.24869133749</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7001,28 +7026,28 @@
         <v>18</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>9089.91800704377</v>
+        <v>8637.55819800001</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>6275.90305206749</v>
+        <v>12151.49096863</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>6992.87984924499</v>
+        <v>8430.21232612498</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>8135.55180300003</v>
+        <v>8374.395685395</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>6869.40717324749</v>
+        <v>8430.21232612498</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>6869.40717324749</v>
+        <v>8568.93904244251</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>7367.01412076499</v>
+        <v>8430.21232612498</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>8146.64725846503</v>
+        <v>8947.90023133128</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7030,28 +7055,28 @@
         <v>19</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>3613.79861410502</v>
+        <v>3571.35174254379</v>
       </c>
       <c r="C12" s="5" t="n">
+        <v>3644.18737555248</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>3599.485019445</v>
       </c>
-      <c r="D12" s="5" t="n">
-        <v>3747.51759493253</v>
-      </c>
       <c r="E12" s="5" t="n">
+        <v>3875.32800106127</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>3875.32800106127</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>3815.30794980003</v>
+      </c>
+      <c r="H12" s="5" t="n">
         <v>3599.485019445</v>
       </c>
-      <c r="F12" s="5" t="n">
-        <v>3815.30794980003</v>
-      </c>
-      <c r="G12" s="5" t="n">
-        <v>3549.4989170475</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <v>3556.76084489254</v>
-      </c>
       <c r="I12" s="5" t="n">
-        <v>3747.51759493253</v>
+        <v>3875.32800106127</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7059,28 +7084,28 @@
         <v>20</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>-6331.6301464325</v>
+        <v>-4652.66915507873</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>-7364.53414455248</v>
+        <v>-6418.0538752675</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>-6068.65805500746</v>
+        <v>-4430.43434809748</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>-5555.19236669501</v>
+        <v>-7803.28609114498</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>-6156.92799643249</v>
+        <v>-4652.66915507873</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>-6418.0538752675</v>
+        <v>-8773.93140440494</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>-6621.90203019875</v>
+        <v>-4430.43434809748</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>-6927.84071813747</v>
+        <v>-7174.88348645502</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7088,28 +7113,28 @@
         <v>21</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>3930.71278343624</v>
+        <v>0</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>2365.28200416504</v>
+        <v>-1416.94233531998</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>-2431.95564293249</v>
+        <v>86.796792697541</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>1253.69332084</v>
+        <v>-3462.01215986999</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1119.75890294376</v>
+        <v>39.3698970000189</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>2230.89931613132</v>
+        <v>-5995.13281816746</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>-3030.95106845125</v>
+        <v>86.796792697541</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>-2575.95885813</v>
+        <v>413.940004841273</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7117,28 +7142,28 @@
         <v>22</v>
       </c>
       <c r="B15" s="5" t="n">
+        <v>8418.37415490751</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>573.083332797553</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>391.605469920031</v>
+      </c>
+      <c r="E15" s="5" t="n">
         <v>4332.05942400001</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>611.095563620001</v>
-      </c>
-      <c r="D15" s="5" t="n">
-        <v>2425.85206453754</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>347.133446467507</v>
       </c>
       <c r="F15" s="5" t="n">
         <v>4332.05942400001</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>2694.77331362</v>
+        <v>4595.33403876002</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>-445.411393034967</v>
+        <v>391.605469920031</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>718.608448306268</v>
+        <v>4332.05942400001</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7146,28 +7171,28 @@
         <v>23</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>-1810.93981197249</v>
+        <v>-1775.52617577875</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>-7505.17656221995</v>
+        <v>-6656.98485223994</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>-4369.5361462137</v>
+        <v>-11949.7259581262</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>-13014.7037844374</v>
+        <v>-10609.7090081462</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>-9158.92831573745</v>
+        <v>-9546.2535622925</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>-12726.2490725349</v>
+        <v>-11745.9909449662</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>-6060.39715562995</v>
+        <v>-11949.7259581262</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>-1479.88641789736</v>
+        <v>-9611.6150365537</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7189,37 +7214,37 @@
       <c r="A19" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="5" t="n">
         <f aca="false">AVERAGE(B2:B16)*4</f>
-        <v>5146.30147198409</v>
-      </c>
-      <c r="C19" s="2" t="n">
+        <v>8470.79268379409</v>
+      </c>
+      <c r="C19" s="5" t="n">
         <f aca="false">AVERAGE(C2:C16)*4</f>
-        <v>205.020319065439</v>
-      </c>
-      <c r="D19" s="2" t="n">
+        <v>2122.47343907775</v>
+      </c>
+      <c r="D19" s="5" t="n">
         <f aca="false">AVERAGE(D2:D16)*4</f>
-        <v>5046.77756975012</v>
-      </c>
-      <c r="E19" s="2" t="n">
+        <v>2162.03323002446</v>
+      </c>
+      <c r="E19" s="5" t="n">
         <f aca="false">AVERAGE(E2:E16)*4</f>
-        <v>2316.48123804376</v>
-      </c>
-      <c r="F19" s="2" t="n">
+        <v>413.167063672443</v>
+      </c>
+      <c r="F19" s="5" t="n">
         <f aca="false">AVERAGE(F2:F16)*4</f>
-        <v>-1264.25715299057</v>
-      </c>
-      <c r="G19" s="2" t="n">
+        <v>-525.014258242583</v>
+      </c>
+      <c r="G19" s="5" t="n">
         <f aca="false">AVERAGE(G2:G16)*4</f>
-        <v>4194.17910159978</v>
-      </c>
-      <c r="H19" s="2" t="n">
+        <v>2315.39967428377</v>
+      </c>
+      <c r="H19" s="5" t="n">
         <f aca="false">AVERAGE(H2:H16)*4</f>
-        <v>332.892119535773</v>
-      </c>
-      <c r="I19" s="2" t="n">
+        <v>4774.39319807012</v>
+      </c>
+      <c r="I19" s="5" t="n">
         <f aca="false">AVERAGE(I2:I16)*4</f>
-        <v>-1648.04868015448</v>
+        <v>1846.65053151477</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7228,35 +7253,35 @@
       </c>
       <c r="B20" s="2" t="n">
         <f aca="false">B19/100000</f>
-        <v>0.0514630147198409</v>
+        <v>0.0847079268379409</v>
       </c>
       <c r="C20" s="2" t="n">
         <f aca="false">C19/100000</f>
-        <v>0.00205020319065439</v>
+        <v>0.0212247343907775</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">D19/100000</f>
-        <v>0.0504677756975012</v>
+        <v>0.0216203323002446</v>
       </c>
       <c r="E20" s="2" t="n">
         <f aca="false">E19/100000</f>
-        <v>0.0231648123804376</v>
+        <v>0.00413167063672443</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">F19/100000</f>
-        <v>-0.0126425715299057</v>
+        <v>-0.00525014258242583</v>
       </c>
       <c r="G20" s="2" t="n">
         <f aca="false">G19/100000</f>
-        <v>0.0419417910159978</v>
+        <v>0.0231539967428377</v>
       </c>
       <c r="H20" s="2" t="n">
         <f aca="false">H19/100000</f>
-        <v>0.00332892119535773</v>
+        <v>0.0477439319807012</v>
       </c>
       <c r="I20" s="2" t="n">
         <f aca="false">I19/100000</f>
-        <v>-0.0164804868015448</v>
+        <v>0.0184665053151477</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7265,35 +7290,35 @@
       </c>
       <c r="B21" s="2" t="n">
         <f aca="false">STDEV(B2:B16)*SQRT(4)</f>
-        <v>9807.36798068197</v>
+        <v>10659.4501131098</v>
       </c>
       <c r="C21" s="2" t="n">
         <f aca="false">STDEV(C2:C16)*SQRT(4)</f>
-        <v>11609.3771504606</v>
+        <v>13321.4156259388</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">STDEV(D2:D16)*SQRT(4)</f>
-        <v>10890.2475458458</v>
+        <v>12764.2397935024</v>
       </c>
       <c r="E21" s="2" t="n">
         <f aca="false">STDEV(E2:E16)*SQRT(4)</f>
-        <v>11659.7427546324</v>
+        <v>11183.5398089395</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">STDEV(F2:F16)*SQRT(4)</f>
-        <v>12103.5422130502</v>
+        <v>11590.0531265203</v>
       </c>
       <c r="G21" s="2" t="n">
         <f aca="false">STDEV(G2:G16)*SQRT(4)</f>
-        <v>11719.4344940034</v>
+        <v>13250.0763406131</v>
       </c>
       <c r="H21" s="2" t="n">
         <f aca="false">STDEV(H2:H16)*SQRT(4)</f>
-        <v>9746.22110511481</v>
+        <v>12866.9822915169</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">STDEV(I2:I16)*SQRT(4)</f>
-        <v>12258.673608396</v>
+        <v>13591.3283160936</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7302,35 +7327,35 @@
       </c>
       <c r="B22" s="2" t="n">
         <f aca="false">B21/100000</f>
-        <v>0.0980736798068197</v>
+        <v>0.106594501131098</v>
       </c>
       <c r="C22" s="2" t="n">
         <f aca="false">C21/100000</f>
-        <v>0.116093771504606</v>
+        <v>0.133214156259388</v>
       </c>
       <c r="D22" s="2" t="n">
         <f aca="false">D21/100000</f>
-        <v>0.108902475458458</v>
+        <v>0.127642397935024</v>
       </c>
       <c r="E22" s="2" t="n">
         <f aca="false">E21/100000</f>
-        <v>0.116597427546324</v>
+        <v>0.111835398089395</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">F21/100000</f>
-        <v>0.121035422130502</v>
+        <v>0.115900531265203</v>
       </c>
       <c r="G22" s="2" t="n">
         <f aca="false">G21/100000</f>
-        <v>0.117194344940034</v>
+        <v>0.132500763406131</v>
       </c>
       <c r="H22" s="2" t="n">
         <f aca="false">H21/100000</f>
-        <v>0.0974622110511481</v>
+        <v>0.128669822915169</v>
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">I21/100000</f>
-        <v>0.12258673608396</v>
+        <v>0.135913283160936</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7339,7 +7364,7 @@
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">COUNTIF(B2:B16,"&gt;0")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">COUNTIF(C2:C16,"&gt;0")</f>
@@ -7347,7 +7372,7 @@
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">COUNTIF(D2:D16,"&gt;0")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">COUNTIF(E2:E16,"&gt;0")</f>
@@ -7359,15 +7384,15 @@
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">COUNTIF(G2:G16,"&gt;0")</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">COUNTIF(H2:H16,"&gt;0")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I23" s="0" t="n">
         <f aca="false">COUNTIF(I2:I16,"&gt;0")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7376,7 +7401,7 @@
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">COUNTIF(B2:B16,"&lt;=0")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">COUNTIF(C2:C16,"&lt;=0")</f>
@@ -7384,7 +7409,7 @@
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">COUNTIF(D2:D16,"&lt;=0")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">COUNTIF(E2:E16,"&lt;=0")</f>
@@ -7396,15 +7421,15 @@
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">COUNTIF(G2:G16,"&lt;=0")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H24" s="0" t="n">
         <f aca="false">COUNTIF(H2:H16,"&lt;=0")</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I24" s="0" t="n">
         <f aca="false">COUNTIF(I2:I16,"&lt;=0")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7413,35 +7438,35 @@
       </c>
       <c r="B25" s="2" t="n">
         <f aca="false">MAX(B2:B16)*4</f>
-        <v>36359.6720281751</v>
+        <v>48581.2665530901</v>
       </c>
       <c r="C25" s="2" t="n">
         <f aca="false">MAX(C2:C16)*4</f>
-        <v>36117.9526141551</v>
+        <v>48605.9638745201</v>
       </c>
       <c r="D25" s="2" t="n">
         <f aca="false">MAX(D2:D16)*4</f>
-        <v>44191.8138006802</v>
+        <v>33720.8493044999</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">MAX(E2:E16)*4</f>
-        <v>33926.9052846351</v>
+        <v>33497.58274158</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">MAX(F2:F16)*4</f>
-        <v>34610.85952236</v>
+        <v>33720.8493044999</v>
       </c>
       <c r="G25" s="2" t="n">
         <f aca="false">MAX(G2:G16)*4</f>
-        <v>33510.0583012051</v>
+        <v>36691.5144036301</v>
       </c>
       <c r="H25" s="2" t="n">
         <f aca="false">MAX(H2:H16)*4</f>
-        <v>30123.5171159651</v>
+        <v>35750.3384805701</v>
       </c>
       <c r="I25" s="2" t="n">
         <f aca="false">MAX(I2:I16)*4</f>
-        <v>33252.7287564502</v>
+        <v>35791.6009253251</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7450,35 +7475,35 @@
       </c>
       <c r="B26" s="2" t="n">
         <f aca="false">MIN(B2:B16)*4</f>
-        <v>-25326.52058573</v>
+        <v>-18610.6766203149</v>
       </c>
       <c r="C26" s="2" t="n">
         <f aca="false">MIN(C2:C16)*4</f>
-        <v>-40650.4074915398</v>
+        <v>-38808.8949065997</v>
       </c>
       <c r="D26" s="2" t="n">
         <f aca="false">MIN(D2:D16)*4</f>
-        <v>-24274.6322200298</v>
+        <v>-47798.9038325048</v>
       </c>
       <c r="E26" s="2" t="n">
         <f aca="false">MIN(E2:E16)*4</f>
-        <v>-52058.8151377498</v>
+        <v>-42438.8360325848</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">MIN(F2:F16)*4</f>
-        <v>-37002.73035909</v>
+        <v>-38185.01424917</v>
       </c>
       <c r="G26" s="2" t="n">
         <f aca="false">MIN(G2:G16)*4</f>
-        <v>-50904.9962901397</v>
+        <v>-46983.9637798649</v>
       </c>
       <c r="H26" s="2" t="n">
         <f aca="false">MIN(H2:H16)*4</f>
-        <v>-26487.608120795</v>
+        <v>-47798.9038325048</v>
       </c>
       <c r="I26" s="2" t="n">
         <f aca="false">MIN(I2:I16)*4</f>
-        <v>-48651.7047639947</v>
+        <v>-40552.3181050297</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7756,21 +7781,21 @@
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="12.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8258,7 +8283,7 @@
       </c>
       <c r="B19" s="2" t="n">
         <f aca="false">AVERAGE(B2:B16)*4</f>
-        <v>-0.0105079245598122</v>
+        <v>-0.0105079245598121</v>
       </c>
       <c r="C19" s="2" t="n">
         <f aca="false">AVERAGE(C2:C16)*4</f>
@@ -8274,7 +8299,7 @@
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">AVERAGE(F2:F16)*4</f>
-        <v>-0.0260102456645451</v>
+        <v>-0.0260102456645452</v>
       </c>
       <c r="G19" s="2" t="n">
         <f aca="false">AVERAGE(G2:G16)*4</f>
@@ -8282,11 +8307,11 @@
       </c>
       <c r="H19" s="2" t="n">
         <f aca="false">AVERAGE(H2:H16)*4</f>
-        <v>-0.0501782586095326</v>
+        <v>-0.0501782586095325</v>
       </c>
       <c r="I19" s="2" t="n">
         <f aca="false">AVERAGE(I2:I16)*4</f>
-        <v>-0.0671196325604122</v>
+        <v>-0.0671196325604121</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8295,7 +8320,7 @@
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">B19*100000</f>
-        <v>-1050.79245598122</v>
+        <v>-1050.79245598121</v>
       </c>
       <c r="C20" s="3" t="n">
         <f aca="false">C19*100000</f>
@@ -8311,7 +8336,7 @@
       </c>
       <c r="F20" s="3" t="n">
         <f aca="false">F19*100000</f>
-        <v>-2601.02456645451</v>
+        <v>-2601.02456645452</v>
       </c>
       <c r="G20" s="3" t="n">
         <f aca="false">G19*100000</f>
@@ -8319,11 +8344,11 @@
       </c>
       <c r="H20" s="3" t="n">
         <f aca="false">H19*100000</f>
-        <v>-5017.82586095326</v>
+        <v>-5017.82586095325</v>
       </c>
       <c r="I20" s="3" t="n">
         <f aca="false">I19*100000</f>
-        <v>-6711.96325604122</v>
+        <v>-6711.96325604121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8406,7 +8431,7 @@
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">B19/B21</f>
-        <v>-0.144653515386522</v>
+        <v>-0.144653515386521</v>
       </c>
       <c r="C23" s="3" t="n">
         <f aca="false">C19/C21</f>
@@ -8422,7 +8447,7 @@
       </c>
       <c r="F23" s="3" t="n">
         <f aca="false">F19/F21</f>
-        <v>-0.357844279182341</v>
+        <v>-0.357844279182342</v>
       </c>
       <c r="G23" s="3" t="n">
         <f aca="false">G19/G21</f>
@@ -8430,7 +8455,7 @@
       </c>
       <c r="H23" s="3" t="n">
         <f aca="false">H19/H21</f>
-        <v>-0.810685194740601</v>
+        <v>-0.8106851947406</v>
       </c>
       <c r="I23" s="3" t="n">
         <f aca="false">I19/I21</f>
@@ -8443,7 +8468,7 @@
       </c>
       <c r="B24" s="3" t="n">
         <f aca="false">B23*100000</f>
-        <v>-14465.3515386522</v>
+        <v>-14465.3515386521</v>
       </c>
       <c r="C24" s="3" t="n">
         <f aca="false">C23*100000</f>
@@ -8459,7 +8484,7 @@
       </c>
       <c r="F24" s="3" t="n">
         <f aca="false">F23*100000</f>
-        <v>-35784.4279182341</v>
+        <v>-35784.4279182342</v>
       </c>
       <c r="G24" s="3" t="n">
         <f aca="false">G23*100000</f>
@@ -8467,7 +8492,7 @@
       </c>
       <c r="H24" s="3" t="n">
         <f aca="false">H23*100000</f>
-        <v>-81068.5194740601</v>
+        <v>-81068.51947406</v>
       </c>
       <c r="I24" s="3" t="n">
         <f aca="false">I23*100000</f>
@@ -9034,21 +9059,21 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9536,11 +9561,11 @@
       </c>
       <c r="B19" s="2" t="n">
         <f aca="false">AVERAGE(B2:B16)*4</f>
-        <v>462.876225288815</v>
+        <v>462.87622528883</v>
       </c>
       <c r="C19" s="2" t="n">
         <f aca="false">AVERAGE(C2:C16)*4</f>
-        <v>-5129.30656498987</v>
+        <v>-5129.30656498986</v>
       </c>
       <c r="D19" s="2" t="n">
         <f aca="false">AVERAGE(D2:D16)*4</f>
@@ -9548,7 +9573,7 @@
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">AVERAGE(E2:E16)*4</f>
-        <v>-4562.58202962787</v>
+        <v>-4562.58202962786</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">AVERAGE(F2:F16)*4</f>
@@ -9556,15 +9581,15 @@
       </c>
       <c r="G19" s="2" t="n">
         <f aca="false">AVERAGE(G2:G16)*4</f>
-        <v>-1777.12411802252</v>
+        <v>-1777.12411802251</v>
       </c>
       <c r="H19" s="2" t="n">
         <f aca="false">AVERAGE(H2:H16)*4</f>
-        <v>-3504.15717968323</v>
+        <v>-3504.15717968322</v>
       </c>
       <c r="I19" s="2" t="n">
         <f aca="false">AVERAGE(I2:I16)*4</f>
-        <v>-5198.29457477119</v>
+        <v>-5198.29457477118</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9573,11 +9598,11 @@
       </c>
       <c r="B20" s="2" t="n">
         <f aca="false">B19/100000</f>
-        <v>0.00462876225288815</v>
+        <v>0.0046287622528883</v>
       </c>
       <c r="C20" s="2" t="n">
         <f aca="false">C19/100000</f>
-        <v>-0.0512930656498987</v>
+        <v>-0.0512930656498986</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">D19/100000</f>
@@ -9585,7 +9610,7 @@
       </c>
       <c r="E20" s="2" t="n">
         <f aca="false">E19/100000</f>
-        <v>-0.0456258202962787</v>
+        <v>-0.0456258202962786</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">F19/100000</f>
@@ -9593,15 +9618,15 @@
       </c>
       <c r="G20" s="2" t="n">
         <f aca="false">G19/100000</f>
-        <v>-0.0177712411802252</v>
+        <v>-0.0177712411802251</v>
       </c>
       <c r="H20" s="2" t="n">
         <f aca="false">H19/100000</f>
-        <v>-0.0350415717968323</v>
+        <v>-0.0350415717968322</v>
       </c>
       <c r="I20" s="2" t="n">
         <f aca="false">I19/100000</f>
-        <v>-0.0519829457477119</v>
+        <v>-0.0519829457477118</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9634,11 +9659,11 @@
       </c>
       <c r="H21" s="2" t="n">
         <f aca="false">STDEV(H2:H16)*SQRT(4)</f>
-        <v>11067.2911504087</v>
+        <v>11067.2911504086</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">STDEV(I2:I16)*SQRT(4)</f>
-        <v>9729.83720116139</v>
+        <v>9729.83720116138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9671,11 +9696,11 @@
       </c>
       <c r="H22" s="2" t="n">
         <f aca="false">H21/100000</f>
-        <v>0.110672911504087</v>
+        <v>0.110672911504086</v>
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">I21/100000</f>
-        <v>0.0972983720116139</v>
+        <v>0.0972983720116138</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9766,11 +9791,11 @@
       </c>
       <c r="D25" s="2" t="n">
         <f aca="false">MAX(D2:D16)*4</f>
-        <v>44895.8092615201</v>
+        <v>44895.80926152</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">MAX(E2:E16)*4</f>
-        <v>44895.8092615201</v>
+        <v>44895.80926152</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">MAX(F2:F16)*4</f>
@@ -9778,11 +9803,11 @@
       </c>
       <c r="G25" s="2" t="n">
         <f aca="false">MAX(G2:G16)*4</f>
-        <v>27118.6697013301</v>
+        <v>27118.6697013302</v>
       </c>
       <c r="H25" s="2" t="n">
         <f aca="false">MAX(H2:H16)*4</f>
-        <v>35772.0417119801</v>
+        <v>35772.04171198</v>
       </c>
       <c r="I25" s="2" t="n">
         <f aca="false">MAX(I2:I16)*4</f>
@@ -9795,19 +9820,19 @@
       </c>
       <c r="B26" s="2" t="n">
         <f aca="false">MIN(B2:B16)*4</f>
-        <v>-76514.8418555698</v>
+        <v>-76514.8418555696</v>
       </c>
       <c r="C26" s="2" t="n">
         <f aca="false">MIN(C2:C16)*4</f>
-        <v>-70710.6157266297</v>
+        <v>-70710.6157266296</v>
       </c>
       <c r="D26" s="2" t="n">
         <f aca="false">MIN(D2:D16)*4</f>
-        <v>-58730.1402939997</v>
+        <v>-58730.1402939996</v>
       </c>
       <c r="E26" s="2" t="n">
         <f aca="false">MIN(E2:E16)*4</f>
-        <v>-72440.0537874998</v>
+        <v>-72440.0537874996</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">MIN(F2:F16)*4</f>
@@ -9819,11 +9844,11 @@
       </c>
       <c r="H26" s="2" t="n">
         <f aca="false">MIN(H2:H16)*4</f>
-        <v>-55821.2406809598</v>
+        <v>-55821.2406809596</v>
       </c>
       <c r="I26" s="2" t="n">
         <f aca="false">MIN(I2:I16)*4</f>
-        <v>-48703.9353771797</v>
+        <v>-48703.9353771796</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10112,11 +10137,14 @@
   </sheetPr>
   <dimension ref="A1:N1693"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85714285714286"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -55968,6 +55996,681 @@
       <c r="H1693" s="3" t="n">
         <f aca="false">AVERAGE(C1693:D1693)</f>
         <v>43.7299995</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.7704081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.0130755506501756</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.0183587547974131</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.0385772902000003</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0.0385772902000003</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0.00586347469182578</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0.00586347469182578</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>-0.0618354832645992</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>-0.0618354832645992</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>-0.0197351509110746</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.0189496725927628</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>-0.000575639994075172</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>-0.0286238770041365</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.0157285709772005</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0.0251096553440005</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0.0181697544209503</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0.0135624516789254</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-0.0411142343933249</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>-0.00944771824717514</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-0.00361464853747515</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>-0.00636665159036251</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>-0.0197348729359001</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>-0.0219594125535749</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>-0.0475699453565999</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>-0.0422076025866749</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>-0.0163325042736123</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>-0.0648688113688494</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>-0.0557496185377249</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.0389137985281752</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>-0.0183049337505496</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>-0.0695170814103745</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>-0.024678611933074</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>-0.0323951578363497</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>-0.0195393921252744</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.037617562126425</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-0.018497421839587</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>-0.0307319450757372</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>-0.0152555778827998</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>-0.0101647775553248</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0.0450631902938255</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0.00119853367785071</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.0226993843243373</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.0229511796826502</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>-0.0168542424188622</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.0311755049271872</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.0201893561099998</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>-0.0204115199994</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0.0246088297288002</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0.0523007004268752</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>-0.0130447476648873</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>-0.0514759660308498</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>-0.0647153162008995</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0.017745331078238</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>-0.00751134364009969</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>-0.00376725506787484</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>-0.0164310477632996</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>-0.0135040480150499</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0.00245818912499975</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>-0.0398581419555373</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.00245818912499975</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0.0389483264813249</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>-0.0104161354286</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>-0.0190802928228252</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>-0.0117854624999999</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>-0.0343649311984752</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0.0460202754383499</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0.00538143471494992</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>-0.0269047527396497</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.00538143471494992</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.0198081203955752</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>-0.0106089230927999</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>-0.0613429674580247</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0.0380097036366001</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0.021026032577988</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>-0.0071141169717749</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>-0.0011790757599749</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>-0.0011790757599749</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.0583805773959758</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0.0225373828047</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0.00205822785470033</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>-0.00825875992364989</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>0.00151042481657528</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0.00136728886997508</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.00352551817352533</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.000867427846000045</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.000720934659474787</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0.000720934659474787</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>-0.00998479468865019</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>-0.00785342313827517</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0.00436754369382479</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>-0.00596149628737504</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.00611456519382485</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.00350330640547474</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>-0.0340531841857496</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>-0.0243851550419496</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.0203218270291504</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>0.0463439438710003</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0.0393071278343624</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.0236528200416504</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.0111975890294376</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.0223089931613132</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0.0471538882134009</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>-0.0523278411285494</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0.0244031132487255</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>-0.0684110328175994</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0.0108053295934499</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>-0.0264043090103502</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.0108053295934499</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>-0.00556753151035018</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>-0.00420331437562482</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0.0121389514590002</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>-0.0449746952403248</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>-0.0316062669910496</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>0.080828294931575</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0.0238859274291004</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0.00734840989392539</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>-0.0283247976740495</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>-0.0977702773434246</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>-0.0832597120210744</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0.0464396443863757</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>0.0256166425070008</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1756</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <f aca="false">AVERAGE(B2:B16)*4</f>
+        <v>0.0352885662979905</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <f aca="false">AVERAGE(C2:C16)*4</f>
+        <v>-0.014124245231196</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <f aca="false">AVERAGE(D2:D16)*4</f>
+        <v>-0.0288170199517561</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <f aca="false">AVERAGE(E2:E16)*4</f>
+        <v>0.0257673425941474</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">AVERAGE(F2:F16)*4</f>
+        <v>-0.0105079245598121</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <f aca="false">AVERAGE(G2:G16)*4</f>
+        <v>-0.066429752462599</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <f aca="false">AVERAGE(H2:H16)*4</f>
+        <v>-0.0260102456645452</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <f aca="false">AVERAGE(I2:I16)*4</f>
+        <v>-0.0329079279929255</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <f aca="false">B19*100000</f>
+        <v>3528.85662979905</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <f aca="false">C19*100000</f>
+        <v>-1412.4245231196</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">D19*100000</f>
+        <v>-2881.70199517561</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <f aca="false">E19*100000</f>
+        <v>2576.73425941474</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <f aca="false">F19*100000</f>
+        <v>-1050.79245598121</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <f aca="false">G19*100000</f>
+        <v>-6642.9752462599</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <f aca="false">H19*100000</f>
+        <v>-2601.02456645452</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <f aca="false">I19*100000</f>
+        <v>-3290.79279929255</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B16,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C16,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D16,"&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E16,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F16,"&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G16,"&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H16,"&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I16,"&gt;0")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B16,"&lt;=0")</f>
+        <v>5</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C16,"&lt;=0")</f>
+        <v>7</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D16,"&lt;=0")</f>
+        <v>8</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E16,"&lt;=0")</f>
+        <v>6</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F16,"&lt;=0")</f>
+        <v>8</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G16,"&lt;=0")</f>
+        <v>10</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H16,"&lt;=0")</f>
+        <v>8</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I16,"&lt;=0")</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrega comparaciones para periodos a la alza
</commit_message>
<xml_diff>
--- a/experimentos/comparacion_experimentos.xlsx
+++ b/experimentos/comparacion_experimentos.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="1778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2579" uniqueCount="1778">
   <si>
     <t>Periodo Prueba</t>
   </si>
@@ -5585,22 +5585,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="B43:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6599,6 +6600,415 @@
       <c r="I31" s="2" t="n">
         <f aca="false">PERCENTILE(I2:I16,0.75)</f>
         <v>4234.65405766875</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>5902.9062404626</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>8314.52144218001</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>8652.3204819688</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>8059.51839429127</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>5902.90624046255</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>8247.55936488004</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>5902.90624046255</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>8148.18349247255</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>4939.8086041775</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>9019.24708919</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>8937.58462014254</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>2062.97415231007</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>2837.4588150438</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>9172.87860090752</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>2812.81805229256</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>3816.31894748378</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>9014.4874283388</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>3848.64440370751</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>8143.67316883748</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>4230.52265156625</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>4230.52265156625</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>4441.22925883128</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>8143.67316883748</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>7988.16109611999</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>7782.4069745875</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>3718.5229022475</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>7782.4069745875</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>3718.5229022475</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>3669.54793836252</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>3718.5229022475</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>7782.4069745875</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>4137.24869133749</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>8478.23209735</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>12151.49096863</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>8430.21232612498</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>8374.395685395</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>9968.99674440628</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>8568.93904244251</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>8430.21232612498</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>8947.90023133128</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>3815.3079498</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>3644.18737555248</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>3599.485019445</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>3875.32800106127</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>3875.32800106127</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>3815.30794980003</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>3599.485019445</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <v>3875.32800106127</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>-3525.6741989175</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>573.083332797553</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>391.605469920031</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>4332.05942400001</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>1750.28772709005</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>4595.33403876002</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>391.605469920031</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>4332.05942400001</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <f aca="false">AVERAGE(B34:B40)</f>
+        <v>5201.06787082842</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <f aca="false">AVERAGE(C34:C40)</f>
+        <v>5895.67107347215</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <f aca="false">AVERAGE(D34:D40)</f>
+        <v>6562.46972300376</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <f aca="false">AVERAGE(E34:E40)</f>
+        <v>4950.47445869591</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <f aca="false">AVERAGE(F34:F40)</f>
+        <v>4605.00687399896</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <f aca="false">AVERAGE(G34:G40)</f>
+        <v>6079.96730826699</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <f aca="false">AVERAGE(H34:H40)</f>
+        <v>5294.72960738144</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <f aca="false">AVERAGE(I34:I40)</f>
+        <v>5892.17141197234</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <f aca="false">MEDIAN(B34:B40)</f>
+        <v>5902.9062404626</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <f aca="false">MEDIAN(C34:C40)</f>
+        <v>3848.64440370751</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <f aca="false">MEDIAN(D34:D40)</f>
+        <v>8143.67316883748</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <f aca="false">MEDIAN(E34:E40)</f>
+        <v>4230.52265156625</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <f aca="false">MEDIAN(F34:F40)</f>
+        <v>3875.32800106127</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <f aca="false">MEDIAN(G34:G40)</f>
+        <v>4595.33403876002</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <f aca="false">MEDIAN(H34:H40)</f>
+        <v>5902.90624046255</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <f aca="false">MEDIAN(I34:I40)</f>
+        <v>4332.05942400001</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <f aca="false">PERCENTILE(B34:B40,0.25)</f>
+        <v>4377.55827698875</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <f aca="false">PERCENTILE(C34:C40,0.25)</f>
+        <v>3681.35513889999</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <f aca="false">PERCENTILE(D34:D40,0.25)</f>
+        <v>5690.94599701625</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <f aca="false">PERCENTILE(E34:E40,0.25)</f>
+        <v>3796.92545165439</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <f aca="false">PERCENTILE(F34:F40,0.25)</f>
+        <v>3253.50337670316</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <f aca="false">PERCENTILE(G34:G40,0.25)</f>
+        <v>4128.26860431566</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <f aca="false">PERCENTILE(H34:H40,0.25)</f>
+        <v>3206.15153586878</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <f aca="false">PERCENTILE(I34:I40,0.25)</f>
+        <v>4006.28834619938</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <f aca="false">PERCENTILE(B34:B40,0.75)</f>
+        <v>8130.31953596875</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <f aca="false">PERCENTILE(C34:C40,0.75)</f>
+        <v>8666.884265685</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <f aca="false">PERCENTILE(D34:D40,0.75)</f>
+        <v>8541.26640404689</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <f aca="false">PERCENTILE(E34:E40,0.75)</f>
+        <v>6195.78890914564</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <f aca="false">PERCENTILE(F34:F40,0.75)</f>
+        <v>5066.7144460144</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <f aca="false">PERCENTILE(G34:G40,0.75)</f>
+        <v>8408.24920366127</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <f aca="false">PERCENTILE(H34:H40,0.75)</f>
+        <v>7963.04007171249</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <f aca="false">PERCENTILE(I34:I40,0.75)</f>
+        <v>8068.17229429627</v>
       </c>
     </row>
   </sheetData>
@@ -6619,13 +7029,13 @@
   </sheetPr>
   <dimension ref="A1:N1693"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52498,17 +52908,17 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="B43:I46 A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.7142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="68.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53173,19 +53583,20 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="1" sqref="B43:I46 A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54747,21 +55158,22 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="B43:I46 A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55989,19 +56401,20 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57205,19 +57618,20 @@
   </sheetPr>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58563,20 +58977,21 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59703,20 +60118,21 @@
   </sheetPr>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61054,20 +61470,21 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62205,21 +62622,22 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43:I46 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>